<commit_message>
edit team back log
</commit_message>
<xml_diff>
--- a/documentation/Team_backlog.xlsx
+++ b/documentation/Team_backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atef\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atef\Desktop\Obstacle-avoidance-car-V1.0\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D2D9C2-A158-4C3E-88B2-46B83BD08663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34513CD-AA9F-409E-A547-0A2C9F9F7810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{87F09DEB-9616-4088-930A-FEC91A9E64DA}"/>
   </bookViews>
@@ -25,22 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>app</t>
-  </si>
-  <si>
-    <t>move</t>
-  </si>
-  <si>
-    <t>display</t>
-  </si>
-  <si>
-    <t>avoidance</t>
-  </si>
-  <si>
-    <t>senseing</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>motor</t>
   </si>
@@ -88,6 +73,57 @@
   </si>
   <si>
     <t>Actual Time</t>
+  </si>
+  <si>
+    <t>16/5    10pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>15/5   10pm</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>keypad</t>
+  </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>f2</t>
+  </si>
+  <si>
+    <t>f3</t>
+  </si>
+  <si>
+    <t>atef</t>
+  </si>
+  <si>
+    <t>khaled</t>
+  </si>
+  <si>
+    <t>buttons</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>anas</t>
+  </si>
+  <si>
+    <t>amr</t>
+  </si>
+  <si>
+    <t>main flow</t>
+  </si>
+  <si>
+    <t>15/5</t>
+  </si>
+  <si>
+    <t>15/5    10pm</t>
   </si>
 </sst>
 </file>
@@ -110,12 +146,30 @@
       <family val="4"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -145,12 +199,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,7 +525,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,157 +539,211 @@
   <sheetData>
     <row r="1" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="B14" s="4"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="B15" s="4"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="B16" s="4"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="B17" s="4"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -644,9 +755,11 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -660,9 +773,11 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -676,9 +791,11 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>

</xml_diff>